<commit_message>
completed create account feature on gantt chart
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -23,6 +23,7 @@
     <definedName function="false" hidden="false" name="TitleRegion..BO60" vbProcedure="false">'Project Planner'!$B$3:$B$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Project Planner'!$3:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'Project Planner'!$3:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Project Planner'!$3:$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -91,18 +92,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0%"/>
-    <numFmt numFmtId="166" formatCode="#,##0"/>
-    <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF404040"/>
       <name val="Corbel"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,100 +120,34 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
+      <sz val="42"/>
+      <color rgb="FF735773"/>
       <name val="Corbel"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Corbel"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF735773"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Corbel"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
-      <color rgb="FF404040"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
+      <sz val="11"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
-      <color rgb="FF735773"/>
-      <name val="Corbel"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF404040"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -222,39 +155,7 @@
       <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF404040"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF404040"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="42"/>
-      <color rgb="FF735773"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF735773"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF404040"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -262,12 +163,14 @@
       <color rgb="FF404040"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -275,9 +178,10 @@
       <color rgb="FF735773"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,110 +190,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFF6DDB9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF735773"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFDCD5DC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF735773"/>
-        <bgColor rgb="FF595959"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE9AB51"/>
-        <bgColor rgb="FFD6BCA8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD6BCA8"/>
-        <bgColor rgb="FFDCD5DC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB5A1B5"/>
-        <bgColor rgb="FFD6BCA8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6DDB9"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDCD5DC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -399,12 +210,8 @@
       <right style="thick">
         <color rgb="FFFFFFFF"/>
       </right>
-      <top style="thick">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -423,49 +230,12 @@
         <color rgb="FFD1871A"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFD1871A"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thick">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thick">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFD1871A"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF735773"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -489,259 +259,98 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="13" borderId="4" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="21" fillId="13" borderId="4" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="5" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="39" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="43" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="49" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="50" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="51" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="13" borderId="4" xfId="45" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="21" fillId="13" borderId="4" xfId="46" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="5" xfId="47" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="6" xfId="42" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="52" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="53" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="53" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="54" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="48" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="3" xfId="44" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="39" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="0" borderId="0" xfId="43" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="% complete" xfId="37" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="38" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Activity" xfId="39" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="40" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Actual legend" xfId="41" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Label" xfId="42" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Percent Complete" xfId="43" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Period Headers" xfId="44" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Period Highlight Control" xfId="45" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Period Value" xfId="46" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Plan legend" xfId="47" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Project Headers" xfId="48" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Title" xfId="49" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Heading 1" xfId="50" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="51" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Heading 2" xfId="52" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Heading 3" xfId="53" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Heading 4" xfId="54" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
       <font>
         <name val="Corbel"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF404040"/>
       </font>
@@ -756,6 +365,7 @@
     <dxf>
       <font>
         <name val="Corbel"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF404040"/>
       </font>
@@ -775,6 +385,7 @@
     <dxf>
       <font>
         <name val="Corbel"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF404040"/>
       </font>
@@ -794,6 +405,7 @@
     <dxf>
       <font>
         <name val="Corbel"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF404040"/>
       </font>
@@ -813,6 +425,7 @@
     <dxf>
       <font>
         <name val="Corbel"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF404040"/>
       </font>
@@ -832,6 +445,7 @@
     <dxf>
       <font>
         <name val="Corbel"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF404040"/>
       </font>
@@ -851,6 +465,7 @@
     <dxf>
       <font>
         <name val="Corbel"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF404040"/>
       </font>
@@ -870,6 +485,7 @@
     <dxf>
       <font>
         <name val="Corbel"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF404040"/>
       </font>
@@ -889,6 +505,7 @@
     <dxf>
       <font>
         <name val="Corbel"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF404040"/>
       </font>
@@ -908,6 +525,7 @@
     <dxf>
       <font>
         <name val="Corbel"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF404040"/>
       </font>
@@ -929,24 +547,24 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFD6BCA8"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF595959"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFE9AB51"/>
       <rgbColor rgb="FF0066CC"/>
@@ -960,13 +578,13 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFF6DDB9"/>
+      <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFF6DDB9"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -978,11 +596,11 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF404040"/>
+      <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF595959"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF404040"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -997,7 +615,7 @@
   <dimension ref="B1:AMJ10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X4" activeCellId="0" sqref="X4"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1005,72 +623,68 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="2" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="15.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="8" style="2" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="971" min="15" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="972" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="8" t="n">
+      <c r="H2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
     </row>
-    <row r="3" s="11" customFormat="true" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="12" t="s">
+    <row r="3" s="8" customFormat="true" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
       <c r="AKJ3" s="0"/>
       <c r="AKK3" s="0"/>
       <c r="AKL3" s="0"/>
@@ -1126,152 +740,152 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="18" t="n">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="18" t="n">
+      <c r="I4" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="18" t="n">
+      <c r="J4" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="K4" s="18" t="n">
+      <c r="K4" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="L4" s="18" t="n">
+      <c r="L4" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="M4" s="18" t="n">
+      <c r="M4" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="N4" s="18" t="n">
+      <c r="N4" s="13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="20" t="n">
+      <c r="C5" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="20" t="n">
+      <c r="D5" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="20" t="n">
+      <c r="E5" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="21" t="n">
+      <c r="F5" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="16" t="n">
         <v>0.01</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="20" t="n">
+      <c r="C6" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="20" t="n">
+      <c r="D6" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="21" t="n">
+      <c r="E6" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="20" t="n">
+      <c r="C7" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="20" t="n">
+      <c r="D7" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="21" t="n">
+      <c r="E7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="20" t="n">
+      <c r="C8" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="20" t="n">
+      <c r="D8" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="E8" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21" t="n">
-        <v>0</v>
+      <c r="E8" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" s="16" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="20" t="n">
+      <c r="C9" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="D9" s="20" t="n">
+      <c r="D9" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="E9" s="20" t="n">
+      <c r="E9" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="21" t="n">
+      <c r="F9" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="16" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="20" t="n">
+      <c r="C10" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="D10" s="20" t="n">
+      <c r="D10" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="21" t="n">
+      <c r="E10" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>